<commit_message>
Fix en UT-03 PD-5
</commit_message>
<xml_diff>
--- a/UT-03/PD5/Comparacion de predicciones RM SCIKIT.xlsx
+++ b/UT-03/PD5/Comparacion de predicciones RM SCIKIT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\IA 1\PDs\UT3\PD5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E2C1621-37FA-43A8-901C-486B2B7B57AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36EF44C-9AE3-4B30-A1B2-306F37A95178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{BA7D8BC6-958C-4419-91BD-38B5E69F9A41}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{BA7D8BC6-958C-4419-91BD-38B5E69F9A41}"/>
   </bookViews>
   <sheets>
     <sheet name="resultadoSCIKITNormalizado (2)" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <definedName name="DatosExternos_6" localSheetId="6">'ResultadoTA6 (2)'!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,10 +164,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2514,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90BB8F8-AD6B-4F22-87F8-F165A28D8A86}">
   <dimension ref="A1:N1842"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2574,12 +2574,12 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <f>COUNTIF(resultadoSCIKITNormalizadoX2__2[[#This Row],[Es Congruente?]]:C1768,"VERDADERO")</f>
+        <f>COUNTIF(C2:C1768,"VERDADERO")</f>
         <v>1368</v>
       </c>
       <c r="G3">
-        <f>COUNTIF(resultadoSCIKITNormalizadoX2__2[[#This Row],[Es Congruente?]]:C1768,"FALSO")</f>
-        <v>398</v>
+        <f>COUNTIF(C2:C1768,"FALSO")</f>
+        <v>399</v>
       </c>
       <c r="L3" s="2"/>
       <c r="N3" s="2"/>
@@ -2596,12 +2596,12 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f>E3/1840</f>
-        <v>0.74347826086956526</v>
-      </c>
-      <c r="G4" s="2">
-        <f>G3/1840</f>
-        <v>0.21630434782608696</v>
+        <f>E3/1766</f>
+        <v>0.77463193657984142</v>
+      </c>
+      <c r="G4" s="3">
+        <f>G3/1766</f>
+        <v>0.22593431483578708</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -28493,7 +28493,7 @@
         <v>3</v>
       </c>
       <c r="C1730" t="b">
-        <f>A1730=B1730</f>
+        <f t="shared" ref="C1730:C1768" si="27">A1730=B1730</f>
         <v>0</v>
       </c>
       <c r="E1730" s="1"/>
@@ -28508,7 +28508,7 @@
         <v>4</v>
       </c>
       <c r="C1731" t="b">
-        <f>A1731=B1731</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1731" s="1"/>
@@ -28523,7 +28523,7 @@
         <v>3</v>
       </c>
       <c r="C1732" t="b">
-        <f>A1732=B1732</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1732" s="1"/>
@@ -28538,7 +28538,7 @@
         <v>3</v>
       </c>
       <c r="C1733" t="b">
-        <f>A1733=B1733</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1733" s="1"/>
@@ -28553,7 +28553,7 @@
         <v>3</v>
       </c>
       <c r="C1734" t="b">
-        <f>A1734=B1734</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1734" s="1"/>
@@ -28568,7 +28568,7 @@
         <v>3</v>
       </c>
       <c r="C1735" t="b">
-        <f>A1735=B1735</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1735" s="1"/>
@@ -28583,7 +28583,7 @@
         <v>3</v>
       </c>
       <c r="C1736" t="b">
-        <f>A1736=B1736</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1736" s="1"/>
@@ -28598,7 +28598,7 @@
         <v>3</v>
       </c>
       <c r="C1737" t="b">
-        <f>A1737=B1737</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1737" s="1"/>
@@ -28613,7 +28613,7 @@
         <v>3</v>
       </c>
       <c r="C1738" t="b">
-        <f>A1738=B1738</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1738" s="1"/>
@@ -28628,7 +28628,7 @@
         <v>3</v>
       </c>
       <c r="C1739" t="b">
-        <f>A1739=B1739</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1739" s="1"/>
@@ -28643,7 +28643,7 @@
         <v>3</v>
       </c>
       <c r="C1740" t="b">
-        <f>A1740=B1740</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1740" s="1"/>
@@ -28658,7 +28658,7 @@
         <v>3</v>
       </c>
       <c r="C1741" t="b">
-        <f>A1741=B1741</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1741" s="1"/>
@@ -28673,7 +28673,7 @@
         <v>3</v>
       </c>
       <c r="C1742" t="b">
-        <f>A1742=B1742</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1742" s="1"/>
@@ -28688,7 +28688,7 @@
         <v>3</v>
       </c>
       <c r="C1743" t="b">
-        <f>A1743=B1743</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1743" s="1"/>
@@ -28703,7 +28703,7 @@
         <v>3</v>
       </c>
       <c r="C1744" t="b">
-        <f>A1744=B1744</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1744" s="1"/>
@@ -28718,7 +28718,7 @@
         <v>4</v>
       </c>
       <c r="C1745" t="b">
-        <f>A1745=B1745</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1745" s="1"/>
@@ -28733,7 +28733,7 @@
         <v>4</v>
       </c>
       <c r="C1746" t="b">
-        <f>A1746=B1746</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1746" s="1"/>
@@ -28748,7 +28748,7 @@
         <v>4</v>
       </c>
       <c r="C1747" t="b">
-        <f>A1747=B1747</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1747" s="1"/>
@@ -28763,7 +28763,7 @@
         <v>3</v>
       </c>
       <c r="C1748" t="b">
-        <f>A1748=B1748</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1748" s="1"/>
@@ -28778,7 +28778,7 @@
         <v>3</v>
       </c>
       <c r="C1749" t="b">
-        <f>A1749=B1749</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1749" s="1"/>
@@ -28793,7 +28793,7 @@
         <v>2</v>
       </c>
       <c r="C1750" t="b">
-        <f>A1750=B1750</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1750" s="1"/>
@@ -28808,7 +28808,7 @@
         <v>3</v>
       </c>
       <c r="C1751" t="b">
-        <f>A1751=B1751</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1751" s="1"/>
@@ -28823,7 +28823,7 @@
         <v>3</v>
       </c>
       <c r="C1752" t="b">
-        <f>A1752=B1752</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1752" s="1"/>
@@ -28838,7 +28838,7 @@
         <v>4</v>
       </c>
       <c r="C1753" t="b">
-        <f>A1753=B1753</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1753" s="1"/>
@@ -28853,7 +28853,7 @@
         <v>4</v>
       </c>
       <c r="C1754" t="b">
-        <f>A1754=B1754</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1754" s="1"/>
@@ -28868,7 +28868,7 @@
         <v>3</v>
       </c>
       <c r="C1755" t="b">
-        <f>A1755=B1755</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1755" s="1"/>
@@ -28883,7 +28883,7 @@
         <v>3</v>
       </c>
       <c r="C1756" t="b">
-        <f>A1756=B1756</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1756" s="1"/>
@@ -28898,7 +28898,7 @@
         <v>3</v>
       </c>
       <c r="C1757" t="b">
-        <f>A1757=B1757</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1757" s="1"/>
@@ -28913,7 +28913,7 @@
         <v>3</v>
       </c>
       <c r="C1758" t="b">
-        <f>A1758=B1758</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1758" s="1"/>
@@ -28928,7 +28928,7 @@
         <v>3</v>
       </c>
       <c r="C1759" t="b">
-        <f>A1759=B1759</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1759" s="1"/>
@@ -28943,7 +28943,7 @@
         <v>2</v>
       </c>
       <c r="C1760" t="b">
-        <f>A1760=B1760</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1760" s="1"/>
@@ -28958,7 +28958,7 @@
         <v>4</v>
       </c>
       <c r="C1761" t="b">
-        <f>A1761=B1761</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1761" s="1"/>
@@ -28973,7 +28973,7 @@
         <v>3</v>
       </c>
       <c r="C1762" t="b">
-        <f>A1762=B1762</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1762" s="1"/>
@@ -28988,7 +28988,7 @@
         <v>3</v>
       </c>
       <c r="C1763" t="b">
-        <f>A1763=B1763</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1763" s="1"/>
@@ -29003,7 +29003,7 @@
         <v>3</v>
       </c>
       <c r="C1764" t="b">
-        <f>A1764=B1764</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1764" s="1"/>
@@ -29018,7 +29018,7 @@
         <v>3</v>
       </c>
       <c r="C1765" t="b">
-        <f>A1765=B1765</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1765" s="1"/>
@@ -29033,7 +29033,7 @@
         <v>3</v>
       </c>
       <c r="C1766" t="b">
-        <f>A1766=B1766</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1766" s="1"/>
@@ -29048,7 +29048,7 @@
         <v>3</v>
       </c>
       <c r="C1767" t="b">
-        <f>A1767=B1767</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E1767" s="1"/>
@@ -29063,7 +29063,7 @@
         <v>3</v>
       </c>
       <c r="C1768" t="b">
-        <f>A1768=B1768</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E1768" s="1"/>
@@ -29591,9 +29591,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>